<commit_message>
Added support to pick specific date with diary post
</commit_message>
<xml_diff>
--- a/static/diary.xlsx
+++ b/static/diary.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -731,10 +731,33 @@
         <v>Worked on my Laravel, TS, PHP, and PHPUnit skills</v>
       </c>
     </row>
+    <row r="31">
+      <c r="A31" t="str">
+        <v>2024-02-28</v>
+      </c>
+      <c r="B31" t="str">
+        <v>Worked on: Fix: Invalid CSV loader stuck, Fix: Additional email sending on inspection close</v>
+      </c>
+      <c r="C31" t="str">
+        <v>Worked on my TS, PHP, and PHPUnit skills</v>
+      </c>
+    </row>
+    <row r="32" xml:space="preserve">
+      <c r="A32" t="str">
+        <v>2024-02-29</v>
+      </c>
+      <c r="B32" t="str" xml:space="preserve">
+        <v xml:space="preserve">Worked on: Feat: Open Weather Integration
+Merged: Feat: Open Weather Integration</v>
+      </c>
+      <c r="C32" t="str">
+        <v>Worked on my  skills</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D30"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D32"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>